<commit_message>
add run_all pipeline and update figures
</commit_message>
<xml_diff>
--- a/Data_Collection_V3.xlsx
+++ b/Data_Collection_V3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danbaby/Library/CloudStorage/Dropbox/1-A/12-Fall 2024/Research/4_Paper_SCMs and Nano and ML/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Desktop/Concrete_ML/Concrete_ML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18186FC1-1EA4-C645-B0CA-4C4E5C3A3F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1978F2C7-8479-A041-BD95-AE51D97CE83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{91031984-F090-7546-9746-8C3AC8ADA00B}"/>
   </bookViews>
@@ -41,43 +41,43 @@
     <t>Data</t>
   </si>
   <si>
-    <t>Cement (kg/m3)</t>
+    <t>Cement</t>
   </si>
   <si>
-    <t>Water (kg/m3)</t>
+    <t>Water</t>
   </si>
   <si>
-    <t>Fine Aggregate (kg/m3)</t>
+    <t>CA</t>
   </si>
   <si>
-    <t>Coarse Aggregate (kg/m3)</t>
+    <t>FA</t>
   </si>
   <si>
-    <t>HRWR (kg/m3)</t>
+    <t>HRWR</t>
   </si>
   <si>
-    <t>Fly ash (kg/m3)</t>
+    <t>FlyAsh</t>
   </si>
   <si>
-    <t>Slag (kg/m3)</t>
+    <t>Slag</t>
   </si>
   <si>
-    <t>Silica Fume (kg/m3)</t>
+    <t>SF</t>
   </si>
   <si>
-    <t>nano-TiO2 (kg/m3)</t>
+    <t>nano-TiO2</t>
   </si>
   <si>
-    <t>nano-SiO2 (kg/m3)</t>
+    <t>nano-SiO2</t>
   </si>
   <si>
-    <t>Concrete Age (days)</t>
+    <t>ConcreteAge</t>
   </si>
   <si>
-    <t>Curing Temperature (degC)</t>
+    <t>TempdegC</t>
   </si>
   <si>
-    <t>Compressive Strength (Mpa)</t>
+    <t>Strength</t>
   </si>
 </sst>
 </file>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36157DF9-4E58-954F-8CD8-677661E42AC6}">
   <dimension ref="A2:N208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,10 +474,10 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>

</xml_diff>